<commit_message>
add 3 times code error retry
</commit_message>
<xml_diff>
--- a/common/data/data.xlsx
+++ b/common/data/data.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\elink\common\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fillsubmit\common\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EDFA2E-2404-4B65-B6C9-5A7491F63F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE0044-4BFB-42D3-A465-D2D20D2AE177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22400" windowHeight="12930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3012" yWindow="2952" windowWidth="17280" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="taskcode" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="ordercode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>分解任务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>汽运任务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>火运计划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>执行结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,18 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>QR20220619002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FJ2041275</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7月1号第二个火运计划</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P12206195437</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -69,6 +45,26 @@
   </si>
   <si>
     <t>P12206216610</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iosapp0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预期结果(0:失败，1:成功)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iosapp00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -76,6 +72,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +111,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -394,46 +396,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.4140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>123456</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -447,34 +477,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDD9EF7-2339-4EE9-A2AC-21F6E9C38C94}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>